<commit_message>
Arreglos varios. Mejoras del consultar facturas
</commit_message>
<xml_diff>
--- a/statics/xlsx/facturas.xlsx
+++ b/statics/xlsx/facturas.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>Facturacion de 2014-02-28 al 2014-02-28</t>
+  </si>
   <si>
     <t>Numero Factura</t>
   </si>
@@ -31,40 +34,19 @@
     <t>Total</t>
   </si>
   <si>
-    <t>2014-02-26</t>
-  </si>
-  <si>
-    <t>16:24:03</t>
-  </si>
-  <si>
-    <t>16:31:42</t>
-  </si>
-  <si>
-    <t>17:32:08</t>
-  </si>
-  <si>
-    <t>17:32:15</t>
+    <t>2014-02-28</t>
+  </si>
+  <si>
+    <t>16:41:48</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>233.00</t>
-  </si>
-  <si>
-    <t>120.00</t>
-  </si>
-  <si>
-    <t>1440.00</t>
-  </si>
-  <si>
-    <t>125.00</t>
-  </si>
-  <si>
-    <t>Total Facturado de 2014-02-26 a 2014-02-28</t>
-  </si>
-  <si>
-    <t>1918.00</t>
+    <t>300.00</t>
+  </si>
+  <si>
+    <t>Total Facturado</t>
   </si>
 </sst>
 </file>
@@ -81,19 +63,25 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,15 +96,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -413,106 +404,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2">
-        <v>7</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2">
+      <c r="E3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Consulta de facturas arreglado
</commit_message>
<xml_diff>
--- a/statics/xlsx/facturas.xlsx
+++ b/statics/xlsx/facturas.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Facturacion de 2014-02-28 al 2014-02-28</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>Facturacion de 2014-03-02 al 2014-03-04</t>
   </si>
   <si>
     <t>Numero Factura</t>
@@ -34,19 +34,28 @@
     <t>Total</t>
   </si>
   <si>
-    <t>2014-02-28</t>
-  </si>
-  <si>
-    <t>16:41:48</t>
+    <t>2014-03-03</t>
+  </si>
+  <si>
+    <t>15:29:57</t>
+  </si>
+  <si>
+    <t>16:37:52</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>300.00</t>
+    <t>100.00</t>
+  </si>
+  <si>
+    <t>167.00</t>
   </si>
   <si>
     <t>Total Facturado</t>
+  </si>
+  <si>
+    <t>267.00</t>
   </si>
 </sst>
 </file>
@@ -404,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,18 +456,35 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>9</v>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>